<commit_message>
Update (Delete Demo Stuff)
</commit_message>
<xml_diff>
--- a/output/observations-summary.xlsx
+++ b/output/observations-summary.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1111" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="273">
   <si>
     <t>Profile</t>
   </si>
@@ -74,6 +74,15 @@
     <t>optional</t>
   </si>
   <si>
+    <t>cde-age-at-diagnosis-of-essential-hypertension</t>
+  </si>
+  <si>
+    <t>CDE Age At Diagnosis Of Essential Hypertension</t>
+  </si>
+  <si>
+    <t>Observation Category Codes#social-history, null#NCIT_C20189, null#NCIT_C171087, null#NCIT_C19332, null#NCIT_C25150, null#NCIT_C156420</t>
+  </si>
+  <si>
     <t>cde-birth-date</t>
   </si>
   <si>
@@ -749,6 +758,12 @@
     <t>CLS OBO NCIT Age</t>
   </si>
   <si>
+    <t>cls-obo-ncit-age-at-diagnosis</t>
+  </si>
+  <si>
+    <t>CLS OBO CMO Age At Diagnosis</t>
+  </si>
+  <si>
     <t>cls-obo-ncit-birth-date</t>
   </si>
   <si>
@@ -816,27 +831,6 @@
   </si>
   <si>
     <t>CLS SNOMED Patient Sex</t>
-  </si>
-  <si>
-    <t>myObservation</t>
-  </si>
-  <si>
-    <t>My Observation Profile</t>
-  </si>
-  <si>
-    <t>LOINC#85354-9</t>
-  </si>
-  <si>
-    <t>Quantityĵ, CodeableConceptĵ</t>
-  </si>
-  <si>
-    <t>LOINC#8480-6</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>LOINC#8462-4</t>
   </si>
 </sst>
 </file>
@@ -970,7 +964,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K101"/>
+  <dimension ref="A1:K100"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -1060,7 +1054,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="s" s="2">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s" s="2">
         <v>16</v>
@@ -1083,19 +1077,19 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s" s="2">
         <v>24</v>
       </c>
-      <c r="B4" t="s" s="2">
+      <c r="C4" t="s" s="2">
         <v>25</v>
       </c>
-      <c r="C4" t="s" s="2">
+      <c r="D4" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s" s="2">
         <v>26</v>
-      </c>
-      <c r="D4" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s" s="2">
-        <v>27</v>
       </c>
       <c r="F4" t="s" s="2">
         <v>16</v>
@@ -1118,19 +1112,19 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s" s="2">
         <v>28</v>
       </c>
-      <c r="B5" t="s" s="2">
+      <c r="C5" t="s" s="2">
         <v>29</v>
       </c>
-      <c r="C5" t="s" s="2">
+      <c r="D5" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s" s="2">
         <v>30</v>
-      </c>
-      <c r="D5" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s" s="2">
-        <v>31</v>
       </c>
       <c r="F5" t="s" s="2">
         <v>16</v>
@@ -1153,19 +1147,19 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s" s="2">
         <v>32</v>
       </c>
-      <c r="B6" t="s" s="2">
+      <c r="C6" t="s" s="2">
         <v>33</v>
       </c>
-      <c r="C6" t="s" s="2">
+      <c r="D6" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s" s="2">
         <v>34</v>
-      </c>
-      <c r="D6" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="E6" t="s" s="2">
-        <v>35</v>
       </c>
       <c r="F6" t="s" s="2">
         <v>16</v>
@@ -1188,19 +1182,19 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s" s="2">
         <v>36</v>
       </c>
-      <c r="B7" t="s" s="2">
+      <c r="C7" t="s" s="2">
         <v>37</v>
       </c>
-      <c r="C7" t="s" s="2">
+      <c r="D7" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s" s="2">
         <v>38</v>
-      </c>
-      <c r="D7" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="E7" t="s" s="2">
-        <v>39</v>
       </c>
       <c r="F7" t="s" s="2">
         <v>16</v>
@@ -1223,13 +1217,13 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="B8" t="s" s="2">
         <v>40</v>
       </c>
-      <c r="B8" t="s" s="2">
+      <c r="C8" t="s" s="2">
         <v>41</v>
-      </c>
-      <c r="C8" t="s" s="2">
-        <v>34</v>
       </c>
       <c r="D8" t="s" s="2">
         <v>14</v>
@@ -1264,13 +1258,13 @@
         <v>44</v>
       </c>
       <c r="C9" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="D9" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s" s="2">
         <v>45</v>
-      </c>
-      <c r="D9" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="E9" t="s" s="2">
-        <v>46</v>
       </c>
       <c r="F9" t="s" s="2">
         <v>16</v>
@@ -1293,13 +1287,13 @@
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="B10" t="s" s="2">
         <v>47</v>
       </c>
-      <c r="B10" t="s" s="2">
+      <c r="C10" t="s" s="2">
         <v>48</v>
-      </c>
-      <c r="C10" t="s" s="2">
-        <v>45</v>
       </c>
       <c r="D10" t="s" s="2">
         <v>14</v>
@@ -1334,13 +1328,13 @@
         <v>51</v>
       </c>
       <c r="C11" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="D11" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E11" t="s" s="2">
         <v>52</v>
-      </c>
-      <c r="D11" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="E11" t="s" s="2">
-        <v>53</v>
       </c>
       <c r="F11" t="s" s="2">
         <v>16</v>
@@ -1363,19 +1357,19 @@
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="B12" t="s" s="2">
         <v>54</v>
       </c>
-      <c r="B12" t="s" s="2">
+      <c r="C12" t="s" s="2">
         <v>55</v>
       </c>
-      <c r="C12" t="s" s="2">
+      <c r="D12" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E12" t="s" s="2">
         <v>56</v>
-      </c>
-      <c r="D12" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="E12" t="s" s="2">
-        <v>57</v>
       </c>
       <c r="F12" t="s" s="2">
         <v>16</v>
@@ -1398,19 +1392,19 @@
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
+        <v>57</v>
+      </c>
+      <c r="B13" t="s" s="2">
         <v>58</v>
       </c>
-      <c r="B13" t="s" s="2">
+      <c r="C13" t="s" s="2">
         <v>59</v>
       </c>
-      <c r="C13" t="s" s="2">
+      <c r="D13" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E13" t="s" s="2">
         <v>60</v>
-      </c>
-      <c r="D13" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="E13" t="s" s="2">
-        <v>61</v>
       </c>
       <c r="F13" t="s" s="2">
         <v>16</v>
@@ -1433,13 +1427,13 @@
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
+        <v>61</v>
+      </c>
+      <c r="B14" t="s" s="2">
         <v>62</v>
       </c>
-      <c r="B14" t="s" s="2">
+      <c r="C14" t="s" s="2">
         <v>63</v>
-      </c>
-      <c r="C14" t="s" s="2">
-        <v>13</v>
       </c>
       <c r="D14" t="s" s="2">
         <v>14</v>
@@ -1451,7 +1445,7 @@
         <v>16</v>
       </c>
       <c r="G14" t="s" s="2">
-        <v>65</v>
+        <v>17</v>
       </c>
       <c r="H14" t="s" s="2">
         <v>18</v>
@@ -1468,10 +1462,10 @@
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="B15" t="s" s="2">
         <v>66</v>
-      </c>
-      <c r="B15" t="s" s="2">
-        <v>67</v>
       </c>
       <c r="C15" t="s" s="2">
         <v>13</v>
@@ -1480,13 +1474,13 @@
         <v>14</v>
       </c>
       <c r="E15" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="F15" t="s" s="2">
+        <v>16</v>
+      </c>
+      <c r="G15" t="s" s="2">
         <v>68</v>
-      </c>
-      <c r="F15" t="s" s="2">
-        <v>16</v>
-      </c>
-      <c r="G15" t="s" s="2">
-        <v>17</v>
       </c>
       <c r="H15" t="s" s="2">
         <v>18</v>
@@ -1509,14 +1503,14 @@
         <v>70</v>
       </c>
       <c r="C16" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="D16" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E16" t="s" s="2">
         <v>71</v>
       </c>
-      <c r="D16" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="E16" t="s" s="2">
-        <v>72</v>
-      </c>
       <c r="F16" t="s" s="2">
         <v>16</v>
       </c>
@@ -1524,7 +1518,7 @@
         <v>17</v>
       </c>
       <c r="H16" t="s" s="2">
-        <v>73</v>
+        <v>18</v>
       </c>
       <c r="I16" t="s" s="2">
         <v>19</v>
@@ -1538,28 +1532,28 @@
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="B17" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="C17" t="s" s="2">
         <v>74</v>
       </c>
-      <c r="B17" t="s" s="2">
+      <c r="D17" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E17" t="s" s="2">
         <v>75</v>
       </c>
-      <c r="C17" t="s" s="2">
+      <c r="F17" t="s" s="2">
+        <v>16</v>
+      </c>
+      <c r="G17" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="H17" t="s" s="2">
         <v>76</v>
-      </c>
-      <c r="D17" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="E17" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="F17" t="s" s="2">
-        <v>16</v>
-      </c>
-      <c r="G17" t="s" s="2">
-        <v>17</v>
-      </c>
-      <c r="H17" t="s" s="2">
-        <v>18</v>
       </c>
       <c r="I17" t="s" s="2">
         <v>19</v>
@@ -1573,19 +1567,19 @@
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="B18" t="s" s="2">
         <v>78</v>
       </c>
-      <c r="B18" t="s" s="2">
+      <c r="C18" t="s" s="2">
         <v>79</v>
       </c>
-      <c r="C18" t="s" s="2">
+      <c r="D18" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E18" t="s" s="2">
         <v>80</v>
-      </c>
-      <c r="D18" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="E18" t="s" s="2">
-        <v>81</v>
       </c>
       <c r="F18" t="s" s="2">
         <v>16</v>
@@ -1608,25 +1602,25 @@
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>14</v>
+        <v>81</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C19" t="s" s="2">
-        <v>14</v>
+        <v>83</v>
       </c>
       <c r="D19" t="s" s="2">
         <v>14</v>
       </c>
       <c r="E19" t="s" s="2">
-        <v>14</v>
+        <v>84</v>
       </c>
       <c r="F19" t="s" s="2">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G19" t="s" s="2">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H19" t="s" s="2">
         <v>18</v>
@@ -1638,7 +1632,7 @@
         <v>14</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>82</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20">
@@ -1646,7 +1640,7 @@
         <v>14</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C20" t="s" s="2">
         <v>14</v>
@@ -1673,7 +1667,7 @@
         <v>14</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21">
@@ -1681,7 +1675,7 @@
         <v>14</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C21" t="s" s="2">
         <v>14</v>
@@ -1708,7 +1702,7 @@
         <v>14</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22">
@@ -1716,7 +1710,7 @@
         <v>14</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C22" t="s" s="2">
         <v>14</v>
@@ -1743,7 +1737,7 @@
         <v>14</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23">
@@ -1751,7 +1745,7 @@
         <v>14</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C23" t="s" s="2">
         <v>14</v>
@@ -1778,7 +1772,7 @@
         <v>14</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24">
@@ -1786,7 +1780,7 @@
         <v>14</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C24" t="s" s="2">
         <v>14</v>
@@ -1813,30 +1807,30 @@
         <v>14</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>14</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="2">
-        <v>86</v>
+        <v>14</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C25" t="s" s="2">
-        <v>88</v>
+        <v>14</v>
       </c>
       <c r="D25" t="s" s="2">
         <v>14</v>
       </c>
       <c r="E25" t="s" s="2">
-        <v>89</v>
+        <v>14</v>
       </c>
       <c r="F25" t="s" s="2">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G25" t="s" s="2">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H25" t="s" s="2">
         <v>18</v>
@@ -1853,19 +1847,19 @@
     </row>
     <row r="26">
       <c r="A26" t="s" s="2">
+        <v>89</v>
+      </c>
+      <c r="B26" t="s" s="2">
         <v>90</v>
       </c>
-      <c r="B26" t="s" s="2">
+      <c r="C26" t="s" s="2">
         <v>91</v>
       </c>
-      <c r="C26" t="s" s="2">
+      <c r="D26" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E26" t="s" s="2">
         <v>92</v>
-      </c>
-      <c r="D26" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="E26" t="s" s="2">
-        <v>93</v>
       </c>
       <c r="F26" t="s" s="2">
         <v>16</v>
@@ -1888,19 +1882,19 @@
     </row>
     <row r="27">
       <c r="A27" t="s" s="2">
+        <v>93</v>
+      </c>
+      <c r="B27" t="s" s="2">
         <v>94</v>
       </c>
-      <c r="B27" t="s" s="2">
+      <c r="C27" t="s" s="2">
         <v>95</v>
       </c>
-      <c r="C27" t="s" s="2">
+      <c r="D27" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E27" t="s" s="2">
         <v>96</v>
-      </c>
-      <c r="D27" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="E27" t="s" s="2">
-        <v>97</v>
       </c>
       <c r="F27" t="s" s="2">
         <v>16</v>
@@ -1923,13 +1917,13 @@
     </row>
     <row r="28">
       <c r="A28" t="s" s="2">
+        <v>97</v>
+      </c>
+      <c r="B28" t="s" s="2">
         <v>98</v>
       </c>
-      <c r="B28" t="s" s="2">
+      <c r="C28" t="s" s="2">
         <v>99</v>
-      </c>
-      <c r="C28" t="s" s="2">
-        <v>96</v>
       </c>
       <c r="D28" t="s" s="2">
         <v>14</v>
@@ -1964,13 +1958,13 @@
         <v>102</v>
       </c>
       <c r="C29" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="D29" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E29" t="s" s="2">
         <v>103</v>
-      </c>
-      <c r="D29" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="E29" t="s" s="2">
-        <v>104</v>
       </c>
       <c r="F29" t="s" s="2">
         <v>16</v>
@@ -1993,19 +1987,19 @@
     </row>
     <row r="30">
       <c r="A30" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="B30" t="s" s="2">
         <v>105</v>
       </c>
-      <c r="B30" t="s" s="2">
+      <c r="C30" t="s" s="2">
         <v>106</v>
       </c>
-      <c r="C30" t="s" s="2">
+      <c r="D30" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E30" t="s" s="2">
         <v>107</v>
-      </c>
-      <c r="D30" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="E30" t="s" s="2">
-        <v>108</v>
       </c>
       <c r="F30" t="s" s="2">
         <v>16</v>
@@ -2028,25 +2022,25 @@
     </row>
     <row r="31">
       <c r="A31" t="s" s="2">
-        <v>14</v>
+        <v>108</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C31" t="s" s="2">
-        <v>14</v>
+        <v>110</v>
       </c>
       <c r="D31" t="s" s="2">
         <v>14</v>
       </c>
       <c r="E31" t="s" s="2">
-        <v>14</v>
+        <v>111</v>
       </c>
       <c r="F31" t="s" s="2">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G31" t="s" s="2">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H31" t="s" s="2">
         <v>18</v>
@@ -2058,7 +2052,7 @@
         <v>14</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>109</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32">
@@ -2066,7 +2060,7 @@
         <v>14</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C32" t="s" s="2">
         <v>14</v>
@@ -2093,7 +2087,7 @@
         <v>14</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="33">
@@ -2101,7 +2095,7 @@
         <v>14</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C33" t="s" s="2">
         <v>14</v>
@@ -2128,7 +2122,7 @@
         <v>14</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34">
@@ -2136,7 +2130,7 @@
         <v>14</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C34" t="s" s="2">
         <v>14</v>
@@ -2163,59 +2157,59 @@
         <v>14</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="2">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C35" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="D35" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E35" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="F35" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="G35" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="H35" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="I35" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="J35" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="K35" t="s" s="2">
         <v>115</v>
-      </c>
-      <c r="D35" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="E35" t="s" s="2">
-        <v>116</v>
-      </c>
-      <c r="F35" t="s" s="2">
-        <v>16</v>
-      </c>
-      <c r="G35" t="s" s="2">
-        <v>17</v>
-      </c>
-      <c r="H35" t="s" s="2">
-        <v>18</v>
-      </c>
-      <c r="I35" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="J35" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="K35" t="s" s="2">
-        <v>14</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="2">
+        <v>116</v>
+      </c>
+      <c r="B36" t="s" s="2">
         <v>117</v>
       </c>
-      <c r="B36" t="s" s="2">
+      <c r="C36" t="s" s="2">
         <v>118</v>
       </c>
-      <c r="C36" t="s" s="2">
+      <c r="D36" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E36" t="s" s="2">
         <v>119</v>
-      </c>
-      <c r="D36" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="E36" t="s" s="2">
-        <v>120</v>
       </c>
       <c r="F36" t="s" s="2">
         <v>16</v>
@@ -2238,19 +2232,19 @@
     </row>
     <row r="37">
       <c r="A37" t="s" s="2">
+        <v>120</v>
+      </c>
+      <c r="B37" t="s" s="2">
         <v>121</v>
       </c>
-      <c r="B37" t="s" s="2">
+      <c r="C37" t="s" s="2">
         <v>122</v>
       </c>
-      <c r="C37" t="s" s="2">
+      <c r="D37" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E37" t="s" s="2">
         <v>123</v>
-      </c>
-      <c r="D37" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="E37" t="s" s="2">
-        <v>124</v>
       </c>
       <c r="F37" t="s" s="2">
         <v>16</v>
@@ -2273,19 +2267,19 @@
     </row>
     <row r="38">
       <c r="A38" t="s" s="2">
+        <v>124</v>
+      </c>
+      <c r="B38" t="s" s="2">
         <v>125</v>
       </c>
-      <c r="B38" t="s" s="2">
+      <c r="C38" t="s" s="2">
         <v>126</v>
       </c>
-      <c r="C38" t="s" s="2">
+      <c r="D38" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E38" t="s" s="2">
         <v>127</v>
-      </c>
-      <c r="D38" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="E38" t="s" s="2">
-        <v>128</v>
       </c>
       <c r="F38" t="s" s="2">
         <v>16</v>
@@ -2308,19 +2302,19 @@
     </row>
     <row r="39">
       <c r="A39" t="s" s="2">
+        <v>128</v>
+      </c>
+      <c r="B39" t="s" s="2">
         <v>129</v>
       </c>
-      <c r="B39" t="s" s="2">
+      <c r="C39" t="s" s="2">
         <v>130</v>
       </c>
-      <c r="C39" t="s" s="2">
+      <c r="D39" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E39" t="s" s="2">
         <v>131</v>
-      </c>
-      <c r="D39" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="E39" t="s" s="2">
-        <v>132</v>
       </c>
       <c r="F39" t="s" s="2">
         <v>16</v>
@@ -2343,19 +2337,19 @@
     </row>
     <row r="40">
       <c r="A40" t="s" s="2">
+        <v>132</v>
+      </c>
+      <c r="B40" t="s" s="2">
         <v>133</v>
       </c>
-      <c r="B40" t="s" s="2">
+      <c r="C40" t="s" s="2">
         <v>134</v>
       </c>
-      <c r="C40" t="s" s="2">
+      <c r="D40" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E40" t="s" s="2">
         <v>135</v>
-      </c>
-      <c r="D40" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="E40" t="s" s="2">
-        <v>136</v>
       </c>
       <c r="F40" t="s" s="2">
         <v>16</v>
@@ -2378,19 +2372,19 @@
     </row>
     <row r="41">
       <c r="A41" t="s" s="2">
+        <v>136</v>
+      </c>
+      <c r="B41" t="s" s="2">
         <v>137</v>
       </c>
-      <c r="B41" t="s" s="2">
+      <c r="C41" t="s" s="2">
         <v>138</v>
       </c>
-      <c r="C41" t="s" s="2">
+      <c r="D41" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E41" t="s" s="2">
         <v>139</v>
-      </c>
-      <c r="D41" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="E41" t="s" s="2">
-        <v>140</v>
       </c>
       <c r="F41" t="s" s="2">
         <v>16</v>
@@ -2413,25 +2407,25 @@
     </row>
     <row r="42">
       <c r="A42" t="s" s="2">
-        <v>14</v>
+        <v>140</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C42" t="s" s="2">
-        <v>14</v>
+        <v>142</v>
       </c>
       <c r="D42" t="s" s="2">
         <v>14</v>
       </c>
       <c r="E42" t="s" s="2">
-        <v>14</v>
+        <v>143</v>
       </c>
       <c r="F42" t="s" s="2">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G42" t="s" s="2">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H42" t="s" s="2">
         <v>18</v>
@@ -2443,7 +2437,7 @@
         <v>14</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>141</v>
+        <v>14</v>
       </c>
     </row>
     <row r="43">
@@ -2451,7 +2445,7 @@
         <v>14</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C43" t="s" s="2">
         <v>14</v>
@@ -2478,7 +2472,7 @@
         <v>14</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="44">
@@ -2486,7 +2480,7 @@
         <v>14</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C44" t="s" s="2">
         <v>14</v>
@@ -2513,59 +2507,59 @@
         <v>14</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="2">
-        <v>144</v>
+        <v>14</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C45" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="D45" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E45" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="F45" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="G45" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="H45" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="I45" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="J45" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="K45" t="s" s="2">
         <v>146</v>
-      </c>
-      <c r="D45" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="E45" t="s" s="2">
-        <v>147</v>
-      </c>
-      <c r="F45" t="s" s="2">
-        <v>16</v>
-      </c>
-      <c r="G45" t="s" s="2">
-        <v>17</v>
-      </c>
-      <c r="H45" t="s" s="2">
-        <v>18</v>
-      </c>
-      <c r="I45" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="J45" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="K45" t="s" s="2">
-        <v>14</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="2">
+        <v>147</v>
+      </c>
+      <c r="B46" t="s" s="2">
         <v>148</v>
       </c>
-      <c r="B46" t="s" s="2">
+      <c r="C46" t="s" s="2">
         <v>149</v>
       </c>
-      <c r="C46" t="s" s="2">
+      <c r="D46" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E46" t="s" s="2">
         <v>150</v>
-      </c>
-      <c r="D46" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="E46" t="s" s="2">
-        <v>151</v>
       </c>
       <c r="F46" t="s" s="2">
         <v>16</v>
@@ -2588,19 +2582,19 @@
     </row>
     <row r="47">
       <c r="A47" t="s" s="2">
+        <v>151</v>
+      </c>
+      <c r="B47" t="s" s="2">
         <v>152</v>
       </c>
-      <c r="B47" t="s" s="2">
+      <c r="C47" t="s" s="2">
         <v>153</v>
       </c>
-      <c r="C47" t="s" s="2">
+      <c r="D47" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E47" t="s" s="2">
         <v>154</v>
-      </c>
-      <c r="D47" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="E47" t="s" s="2">
-        <v>15</v>
       </c>
       <c r="F47" t="s" s="2">
         <v>16</v>
@@ -2635,7 +2629,7 @@
         <v>14</v>
       </c>
       <c r="E48" t="s" s="2">
-        <v>158</v>
+        <v>15</v>
       </c>
       <c r="F48" t="s" s="2">
         <v>16</v>
@@ -2658,19 +2652,19 @@
     </row>
     <row r="49">
       <c r="A49" t="s" s="2">
+        <v>158</v>
+      </c>
+      <c r="B49" t="s" s="2">
         <v>159</v>
       </c>
-      <c r="B49" t="s" s="2">
+      <c r="C49" t="s" s="2">
         <v>160</v>
       </c>
-      <c r="C49" t="s" s="2">
+      <c r="D49" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E49" t="s" s="2">
         <v>161</v>
-      </c>
-      <c r="D49" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="E49" t="s" s="2">
-        <v>162</v>
       </c>
       <c r="F49" t="s" s="2">
         <v>16</v>
@@ -2693,19 +2687,19 @@
     </row>
     <row r="50">
       <c r="A50" t="s" s="2">
+        <v>162</v>
+      </c>
+      <c r="B50" t="s" s="2">
         <v>163</v>
       </c>
-      <c r="B50" t="s" s="2">
+      <c r="C50" t="s" s="2">
         <v>164</v>
       </c>
-      <c r="C50" t="s" s="2">
+      <c r="D50" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E50" t="s" s="2">
         <v>165</v>
-      </c>
-      <c r="D50" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="E50" t="s" s="2">
-        <v>166</v>
       </c>
       <c r="F50" t="s" s="2">
         <v>16</v>
@@ -2728,25 +2722,25 @@
     </row>
     <row r="51">
       <c r="A51" t="s" s="2">
-        <v>14</v>
+        <v>166</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C51" t="s" s="2">
-        <v>14</v>
+        <v>168</v>
       </c>
       <c r="D51" t="s" s="2">
         <v>14</v>
       </c>
       <c r="E51" t="s" s="2">
-        <v>14</v>
+        <v>169</v>
       </c>
       <c r="F51" t="s" s="2">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G51" t="s" s="2">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H51" t="s" s="2">
         <v>18</v>
@@ -2758,7 +2752,7 @@
         <v>14</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>167</v>
+        <v>14</v>
       </c>
     </row>
     <row r="52">
@@ -2766,7 +2760,7 @@
         <v>14</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C52" t="s" s="2">
         <v>14</v>
@@ -2793,7 +2787,7 @@
         <v>14</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="53">
@@ -2801,7 +2795,7 @@
         <v>14</v>
       </c>
       <c r="B53" t="s" s="2">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C53" t="s" s="2">
         <v>14</v>
@@ -2828,7 +2822,7 @@
         <v>14</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="54">
@@ -2836,7 +2830,7 @@
         <v>14</v>
       </c>
       <c r="B54" t="s" s="2">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C54" t="s" s="2">
         <v>14</v>
@@ -2863,18 +2857,18 @@
         <v>14</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="2">
-        <v>171</v>
+        <v>14</v>
       </c>
       <c r="B55" t="s" s="2">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C55" t="s" s="2">
-        <v>165</v>
+        <v>14</v>
       </c>
       <c r="D55" t="s" s="2">
         <v>14</v>
@@ -2883,10 +2877,10 @@
         <v>14</v>
       </c>
       <c r="F55" t="s" s="2">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G55" t="s" s="2">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H55" t="s" s="2">
         <v>18</v>
@@ -2898,24 +2892,24 @@
         <v>14</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>14</v>
+        <v>173</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="2">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B56" t="s" s="2">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C56" t="s" s="2">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="D56" t="s" s="2">
         <v>14</v>
       </c>
       <c r="E56" t="s" s="2">
-        <v>57</v>
+        <v>14</v>
       </c>
       <c r="F56" t="s" s="2">
         <v>16</v>
@@ -2950,7 +2944,7 @@
         <v>14</v>
       </c>
       <c r="E57" t="s" s="2">
-        <v>179</v>
+        <v>60</v>
       </c>
       <c r="F57" t="s" s="2">
         <v>16</v>
@@ -2973,19 +2967,19 @@
     </row>
     <row r="58">
       <c r="A58" t="s" s="2">
+        <v>179</v>
+      </c>
+      <c r="B58" t="s" s="2">
         <v>180</v>
       </c>
-      <c r="B58" t="s" s="2">
+      <c r="C58" t="s" s="2">
         <v>181</v>
       </c>
-      <c r="C58" t="s" s="2">
+      <c r="D58" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E58" t="s" s="2">
         <v>182</v>
-      </c>
-      <c r="D58" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="E58" t="s" s="2">
-        <v>183</v>
       </c>
       <c r="F58" t="s" s="2">
         <v>16</v>
@@ -3008,19 +3002,19 @@
     </row>
     <row r="59">
       <c r="A59" t="s" s="2">
+        <v>183</v>
+      </c>
+      <c r="B59" t="s" s="2">
         <v>184</v>
       </c>
-      <c r="B59" t="s" s="2">
+      <c r="C59" t="s" s="2">
         <v>185</v>
       </c>
-      <c r="C59" t="s" s="2">
-        <v>45</v>
-      </c>
       <c r="D59" t="s" s="2">
         <v>14</v>
       </c>
       <c r="E59" t="s" s="2">
-        <v>14</v>
+        <v>186</v>
       </c>
       <c r="F59" t="s" s="2">
         <v>16</v>
@@ -3043,13 +3037,13 @@
     </row>
     <row r="60">
       <c r="A60" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B60" t="s" s="2">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C60" t="s" s="2">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D60" t="s" s="2">
         <v>14</v>
@@ -3078,13 +3072,13 @@
     </row>
     <row r="61">
       <c r="A61" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B61" t="s" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C61" t="s" s="2">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D61" t="s" s="2">
         <v>14</v>
@@ -3113,13 +3107,13 @@
     </row>
     <row r="62">
       <c r="A62" t="s" s="2">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B62" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C62" t="s" s="2">
-        <v>192</v>
+        <v>59</v>
       </c>
       <c r="D62" t="s" s="2">
         <v>14</v>
@@ -3154,7 +3148,7 @@
         <v>194</v>
       </c>
       <c r="C63" t="s" s="2">
-        <v>88</v>
+        <v>195</v>
       </c>
       <c r="D63" t="s" s="2">
         <v>14</v>
@@ -3183,13 +3177,13 @@
     </row>
     <row r="64">
       <c r="A64" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B64" t="s" s="2">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C64" t="s" s="2">
-        <v>119</v>
+        <v>91</v>
       </c>
       <c r="D64" t="s" s="2">
         <v>14</v>
@@ -3218,13 +3212,13 @@
     </row>
     <row r="65">
       <c r="A65" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B65" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C65" t="s" s="2">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D65" t="s" s="2">
         <v>14</v>
@@ -3253,13 +3247,13 @@
     </row>
     <row r="66">
       <c r="A66" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B66" t="s" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C66" t="s" s="2">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D66" t="s" s="2">
         <v>14</v>
@@ -3288,13 +3282,13 @@
     </row>
     <row r="67">
       <c r="A67" t="s" s="2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B67" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C67" t="s" s="2">
-        <v>203</v>
+        <v>138</v>
       </c>
       <c r="D67" t="s" s="2">
         <v>14</v>
@@ -3329,7 +3323,7 @@
         <v>205</v>
       </c>
       <c r="C68" t="s" s="2">
-        <v>146</v>
+        <v>206</v>
       </c>
       <c r="D68" t="s" s="2">
         <v>14</v>
@@ -3358,13 +3352,13 @@
     </row>
     <row r="69">
       <c r="A69" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B69" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C69" t="s" s="2">
-        <v>175</v>
+        <v>149</v>
       </c>
       <c r="D69" t="s" s="2">
         <v>14</v>
@@ -3393,13 +3387,13 @@
     </row>
     <row r="70">
       <c r="A70" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B70" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C70" t="s" s="2">
-        <v>34</v>
+        <v>178</v>
       </c>
       <c r="D70" t="s" s="2">
         <v>14</v>
@@ -3428,13 +3422,13 @@
     </row>
     <row r="71">
       <c r="A71" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B71" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C71" t="s" s="2">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D71" t="s" s="2">
         <v>14</v>
@@ -3463,13 +3457,13 @@
     </row>
     <row r="72">
       <c r="A72" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B72" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C72" t="s" s="2">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D72" t="s" s="2">
         <v>14</v>
@@ -3498,13 +3492,13 @@
     </row>
     <row r="73">
       <c r="A73" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B73" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C73" t="s" s="2">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="D73" t="s" s="2">
         <v>14</v>
@@ -3533,13 +3527,13 @@
     </row>
     <row r="74">
       <c r="A74" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B74" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C74" t="s" s="2">
-        <v>92</v>
+        <v>29</v>
       </c>
       <c r="D74" t="s" s="2">
         <v>14</v>
@@ -3568,13 +3562,13 @@
     </row>
     <row r="75">
       <c r="A75" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B75" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C75" t="s" s="2">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D75" t="s" s="2">
         <v>14</v>
@@ -3603,13 +3597,13 @@
     </row>
     <row r="76">
       <c r="A76" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B76" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C76" t="s" s="2">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D76" t="s" s="2">
         <v>14</v>
@@ -3638,13 +3632,13 @@
     </row>
     <row r="77">
       <c r="A77" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B77" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C77" t="s" s="2">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D77" t="s" s="2">
         <v>14</v>
@@ -3673,13 +3667,13 @@
     </row>
     <row r="78">
       <c r="A78" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B78" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C78" t="s" s="2">
-        <v>226</v>
+        <v>106</v>
       </c>
       <c r="D78" t="s" s="2">
         <v>14</v>
@@ -3714,7 +3708,7 @@
         <v>228</v>
       </c>
       <c r="C79" t="s" s="2">
-        <v>123</v>
+        <v>229</v>
       </c>
       <c r="D79" t="s" s="2">
         <v>14</v>
@@ -3743,13 +3737,13 @@
     </row>
     <row r="80">
       <c r="A80" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B80" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C80" t="s" s="2">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D80" t="s" s="2">
         <v>14</v>
@@ -3778,13 +3772,13 @@
     </row>
     <row r="81">
       <c r="A81" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B81" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C81" t="s" s="2">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="D81" t="s" s="2">
         <v>14</v>
@@ -3813,13 +3807,13 @@
     </row>
     <row r="82">
       <c r="A82" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B82" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C82" t="s" s="2">
-        <v>76</v>
+        <v>153</v>
       </c>
       <c r="D82" t="s" s="2">
         <v>14</v>
@@ -3848,13 +3842,13 @@
     </row>
     <row r="83">
       <c r="A83" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B83" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C83" t="s" s="2">
-        <v>30</v>
+        <v>79</v>
       </c>
       <c r="D83" t="s" s="2">
         <v>14</v>
@@ -3883,13 +3877,13 @@
     </row>
     <row r="84">
       <c r="A84" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B84" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C84" t="s" s="2">
-        <v>107</v>
+        <v>33</v>
       </c>
       <c r="D84" t="s" s="2">
         <v>14</v>
@@ -3918,13 +3912,13 @@
     </row>
     <row r="85">
       <c r="A85" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B85" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C85" t="s" s="2">
-        <v>182</v>
+        <v>110</v>
       </c>
       <c r="D85" t="s" s="2">
         <v>14</v>
@@ -3953,13 +3947,13 @@
     </row>
     <row r="86">
       <c r="A86" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B86" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C86" t="s" s="2">
-        <v>115</v>
+        <v>185</v>
       </c>
       <c r="D86" t="s" s="2">
         <v>14</v>
@@ -3988,13 +3982,13 @@
     </row>
     <row r="87">
       <c r="A87" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B87" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C87" t="s" s="2">
-        <v>13</v>
+        <v>118</v>
       </c>
       <c r="D87" t="s" s="2">
         <v>14</v>
@@ -4023,13 +4017,13 @@
     </row>
     <row r="88">
       <c r="A88" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B88" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C88" t="s" s="2">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D88" t="s" s="2">
         <v>14</v>
@@ -4058,13 +4052,13 @@
     </row>
     <row r="89">
       <c r="A89" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B89" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C89" t="s" s="2">
-        <v>249</v>
+        <v>22</v>
       </c>
       <c r="D89" t="s" s="2">
         <v>14</v>
@@ -4099,7 +4093,7 @@
         <v>251</v>
       </c>
       <c r="C90" t="s" s="2">
-        <v>71</v>
+        <v>25</v>
       </c>
       <c r="D90" t="s" s="2">
         <v>14</v>
@@ -4134,7 +4128,7 @@
         <v>253</v>
       </c>
       <c r="C91" t="s" s="2">
-        <v>178</v>
+        <v>254</v>
       </c>
       <c r="D91" t="s" s="2">
         <v>14</v>
@@ -4163,13 +4157,13 @@
     </row>
     <row r="92">
       <c r="A92" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B92" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C92" t="s" s="2">
-        <v>157</v>
+        <v>74</v>
       </c>
       <c r="D92" t="s" s="2">
         <v>14</v>
@@ -4198,13 +4192,13 @@
     </row>
     <row r="93">
       <c r="A93" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B93" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C93" t="s" s="2">
-        <v>60</v>
+        <v>181</v>
       </c>
       <c r="D93" t="s" s="2">
         <v>14</v>
@@ -4233,13 +4227,13 @@
     </row>
     <row r="94">
       <c r="A94" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B94" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C94" t="s" s="2">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="D94" t="s" s="2">
         <v>14</v>
@@ -4268,13 +4262,13 @@
     </row>
     <row r="95">
       <c r="A95" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B95" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C95" t="s" s="2">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="D95" t="s" s="2">
         <v>14</v>
@@ -4303,13 +4297,13 @@
     </row>
     <row r="96">
       <c r="A96" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B96" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C96" t="s" s="2">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="D96" t="s" s="2">
         <v>14</v>
@@ -4338,13 +4332,13 @@
     </row>
     <row r="97">
       <c r="A97" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B97" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C97" t="s" s="2">
-        <v>161</v>
+        <v>83</v>
       </c>
       <c r="D97" t="s" s="2">
         <v>14</v>
@@ -4373,13 +4367,13 @@
     </row>
     <row r="98">
       <c r="A98" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B98" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C98" t="s" s="2">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="D98" t="s" s="2">
         <v>14</v>
@@ -4408,28 +4402,28 @@
     </row>
     <row r="99">
       <c r="A99" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B99" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C99" t="s" s="2">
-        <v>14</v>
+        <v>164</v>
       </c>
       <c r="D99" t="s" s="2">
         <v>14</v>
       </c>
       <c r="E99" t="s" s="2">
-        <v>270</v>
+        <v>14</v>
       </c>
       <c r="F99" t="s" s="2">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G99" t="s" s="2">
         <v>17</v>
       </c>
       <c r="H99" t="s" s="2">
-        <v>271</v>
+        <v>18</v>
       </c>
       <c r="I99" t="s" s="2">
         <v>19</v>
@@ -4443,28 +4437,28 @@
     </row>
     <row r="100">
       <c r="A100" t="s" s="2">
-        <v>14</v>
+        <v>271</v>
       </c>
       <c r="B100" t="s" s="2">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="C100" t="s" s="2">
-        <v>14</v>
+        <v>142</v>
       </c>
       <c r="D100" t="s" s="2">
         <v>14</v>
       </c>
       <c r="E100" t="s" s="2">
-        <v>272</v>
+        <v>14</v>
       </c>
       <c r="F100" t="s" s="2">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G100" t="s" s="2">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H100" t="s" s="2">
-        <v>273</v>
+        <v>18</v>
       </c>
       <c r="I100" t="s" s="2">
         <v>19</v>
@@ -4473,41 +4467,6 @@
         <v>14</v>
       </c>
       <c r="K100" t="s" s="2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="B101" t="s" s="2">
-        <v>269</v>
-      </c>
-      <c r="C101" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="D101" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="E101" t="s" s="2">
-        <v>274</v>
-      </c>
-      <c r="F101" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="G101" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="H101" t="s" s="2">
-        <v>273</v>
-      </c>
-      <c r="I101" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="J101" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="K101" t="s" s="2">
         <v>14</v>
       </c>
     </row>

</xml_diff>